<commit_message>
Drools Decision tables test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/com/tvajjala/drools/student_grade.xlsx
+++ b/src/main/resources/com/tvajjala/drools/student_grade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>RuleSet</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>$std.setGrade($param);drools.halt();</t>
+  </si>
+  <si>
+    <t>AGENDA-GROUP</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agenda </t>
   </si>
 </sst>
 </file>
@@ -145,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -228,15 +249,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,9 +266,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E19"/>
+  <dimension ref="B1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -598,138 +623,157 @@
     <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="18">
+    <row r="1" spans="2:6" ht="18">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="2:5" ht="18">
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="2:6" ht="18">
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="2:5" ht="18">
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:6" ht="18">
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="2:5">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="2:6">
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="6" spans="2:5" ht="18">
-      <c r="B6" s="8" t="s">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="6" spans="2:6" ht="18">
+      <c r="B6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="2:5">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="2:6">
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:5">
+      <c r="F7" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
       <c r="B8" s="7"/>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="C9" s="19" t="s">
+      <c r="D8" s="20"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="C9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="2:5">
+      <c r="F9" s="24"/>
+    </row>
+    <row r="10" spans="2:6">
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:5">
+      <c r="F10" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="10">
         <v>900</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="10">
         <v>95.5</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="2:5">
+      <c r="F11" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="10">
         <v>700</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="10">
         <v>80.5</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="2:5">
+      <c r="F12" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="10">
         <v>500</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="10">
         <v>70.5</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="12" t="s">
         <v>20</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:2">
@@ -737,12 +781,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B6:F6"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>